<commit_message>
date + anciennete + age
</commit_message>
<xml_diff>
--- a/Dictionnaire de données.xlsx
+++ b/Dictionnaire de données.xlsx
@@ -165,7 +165,7 @@
   <si>
     <t xml:space="preserve">Description : Indique si le client est une personne physique ou morale.
 Utilité : Pertinent pour différencier comportements et risques.
-Conserver ? Oui.</t>
+Conserver ? Non car information déjà comprise dans la variable AGEPRS</t>
   </si>
   <si>
     <t xml:space="preserve">Sexe du client : Non autorisé car cela peut induire des biais discriminatoires.</t>
@@ -897,7 +897,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -931,19 +931,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin">
-        <color rgb="FF9DC3E6"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF9DC3E6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF9DC3E6"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -986,12 +973,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1075,24 +1066,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1228,1460 +1211,1460 @@
   </sheetPr>
   <dimension ref="B1:J123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="104.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="25.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="104.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="n">
+      <c r="E2" s="4" t="n">
         <v>708</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>34188</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4" t="n">
+      <c r="D3" s="5"/>
+      <c r="E3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="n">
+      <c r="H3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6" t="n">
+      <c r="D4" s="5"/>
+      <c r="E4" s="7" t="n">
         <v>202301</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <v>6</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6" t="n">
+      <c r="H4" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="7" t="n">
         <v>67</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="5" t="n">
         <v>80</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="6" t="n">
+      <c r="H5" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6" t="n">
+      <c r="D6" s="5"/>
+      <c r="E6" s="7" t="n">
         <v>576</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="5" t="n">
         <v>750</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="6" t="n">
+      <c r="H6" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="5" t="n">
         <v>83</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="9" t="s">
+      <c r="H7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="5"/>
+      <c r="E8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="6" t="n">
+      <c r="H8" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="0" t="s">
+      <c r="H9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="4" t="s">
+    <row r="10" customFormat="false" ht="36.05" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="5"/>
+      <c r="E10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="4" t="n">
+      <c r="F10" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="0" t="s">
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="6" t="n">
+      <c r="D11" s="5"/>
+      <c r="E11" s="7" t="n">
         <v>321443</v>
       </c>
-      <c r="F11" s="4" t="n">
+      <c r="F11" s="5" t="n">
         <v>30744</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="0" t="s">
+      <c r="H11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="6" t="n">
+      <c r="D12" s="5"/>
+      <c r="E12" s="7" t="n">
         <v>123</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="5" t="n">
         <v>656</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="0" t="s">
+      <c r="H12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="6" t="n">
+      <c r="D13" s="5"/>
+      <c r="E13" s="7" t="n">
         <v>189</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="5" t="n">
         <v>621</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="0" t="s">
+      <c r="H13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="6" t="n">
+      <c r="D14" s="5"/>
+      <c r="E14" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="5" t="n">
         <v>897</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H14" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="0" t="s">
+      <c r="H14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4" t="n">
+      <c r="D15" s="5"/>
+      <c r="E15" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5" t="n">
         <v>222</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="H15" s="6" t="n">
+      <c r="H15" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4" t="n">
+      <c r="D16" s="5"/>
+      <c r="E16" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5" t="n">
         <v>223</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="6" t="n">
+      <c r="H16" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="43.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="6" t="n">
+      <c r="D17" s="5"/>
+      <c r="E17" s="7" t="n">
         <v>10252000</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <v>6586</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="H17" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="J17" s="11" t="s">
+      <c r="H17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="6" t="n">
+      <c r="D18" s="5"/>
+      <c r="E18" s="7" t="n">
         <v>10205333</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="5" t="n">
         <v>16404</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="6" t="n">
+      <c r="H18" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="6" t="n">
+      <c r="D19" s="5"/>
+      <c r="E19" s="7" t="n">
         <v>10031666</v>
       </c>
-      <c r="F19" s="4" t="n">
+      <c r="F19" s="5" t="n">
         <v>16525</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H19" s="6" t="n">
+      <c r="H19" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="6" t="n">
+      <c r="D20" s="5"/>
+      <c r="E20" s="7" t="n">
         <v>7019332</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="5" t="n">
         <v>16546</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H20" s="6" t="n">
+      <c r="H20" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="6" t="n">
+      <c r="D21" s="5"/>
+      <c r="E21" s="7" t="n">
         <v>5749333</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="5" t="n">
         <v>16365</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="6" t="n">
+      <c r="G21" s="15"/>
+      <c r="H21" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="6" t="n">
+      <c r="D22" s="5"/>
+      <c r="E22" s="7" t="n">
         <v>5309666</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <v>16191</v>
       </c>
-      <c r="G22" s="15"/>
-      <c r="H22" s="6" t="n">
+      <c r="G22" s="16"/>
+      <c r="H22" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" s="4" t="n">
+      <c r="D23" s="5"/>
+      <c r="E23" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5" t="n">
         <v>89</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="H23" s="6" t="n">
+      <c r="H23" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="4"/>
-      <c r="E24" s="6" t="n">
+      <c r="D24" s="5"/>
+      <c r="E24" s="7" t="n">
         <v>10252000</v>
       </c>
-      <c r="F24" s="4" t="n">
+      <c r="F24" s="5" t="n">
         <v>7459</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="6" t="n">
+      <c r="H24" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" s="4" t="n">
+      <c r="D25" s="5"/>
+      <c r="E25" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5" t="n">
         <v>133</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="6" t="n">
+      <c r="H25" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="4"/>
-      <c r="E26" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" s="4" t="n">
+      <c r="D26" s="5"/>
+      <c r="E26" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5" t="n">
         <v>3498</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H26" s="6" t="n">
+      <c r="H26" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D27" s="4"/>
-      <c r="E27" s="6" t="n">
+      <c r="D27" s="5"/>
+      <c r="E27" s="7" t="n">
         <v>13245000</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="5" t="n">
         <v>15378</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H27" s="6" t="n">
+      <c r="H27" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="4"/>
-      <c r="E28" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4" t="n">
+      <c r="D28" s="5"/>
+      <c r="E28" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5" t="n">
         <v>8700</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="H28" s="6" t="n">
+      <c r="H28" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="4"/>
-      <c r="E29" s="6" t="n">
+      <c r="D29" s="5"/>
+      <c r="E29" s="7" t="n">
         <v>1045944</v>
       </c>
-      <c r="F29" s="4" t="n">
+      <c r="F29" s="5" t="n">
         <v>61266</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H29" s="6" t="n">
+      <c r="H29" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="6" t="n">
+      <c r="D30" s="5"/>
+      <c r="E30" s="7" t="n">
         <v>951063</v>
       </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="5" t="n">
         <v>183331</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="G30" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="H30" s="6" t="n">
+      <c r="H30" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="4"/>
-      <c r="E31" s="6" t="n">
+      <c r="D31" s="5"/>
+      <c r="E31" s="7" t="n">
         <v>-35094</v>
       </c>
-      <c r="F31" s="4" t="n">
+      <c r="F31" s="5" t="n">
         <v>14955</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H31" s="6" t="n">
+      <c r="H31" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="6" t="n">
+      <c r="D32" s="5"/>
+      <c r="E32" s="7" t="n">
         <v>-2924</v>
       </c>
-      <c r="F32" s="4" t="n">
+      <c r="F32" s="5" t="n">
         <v>37766</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="H32" s="6" t="n">
+      <c r="H32" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6" t="n">
+      <c r="D33" s="5"/>
+      <c r="E33" s="7" t="n">
         <v>15000</v>
       </c>
-      <c r="F33" s="4" t="n">
+      <c r="F33" s="5" t="n">
         <v>49330</v>
       </c>
-      <c r="G33" s="7" t="s">
+      <c r="G33" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="H33" s="6" t="n">
+      <c r="H33" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="6" t="n">
+      <c r="D34" s="5"/>
+      <c r="E34" s="7" t="n">
         <v>10833</v>
       </c>
-      <c r="F34" s="4" t="n">
+      <c r="F34" s="5" t="n">
         <v>143578</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="G34" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="H34" s="6" t="n">
+      <c r="H34" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="6" t="n">
+      <c r="D35" s="5"/>
+      <c r="E35" s="7" t="n">
         <v>164</v>
       </c>
-      <c r="F35" s="4" t="n">
+      <c r="F35" s="5" t="n">
         <v>549</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G35" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H35" s="6" t="n">
+      <c r="H35" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="6" t="n">
+      <c r="D36" s="5"/>
+      <c r="E36" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F36" s="4" t="n">
+      <c r="F36" s="5" t="n">
         <v>263</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G36" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="H36" s="6" t="n">
+      <c r="H36" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="4"/>
-      <c r="E37" s="6" t="n">
+      <c r="D37" s="5"/>
+      <c r="E37" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F37" s="4" t="n">
+      <c r="F37" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G37" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="H37" s="6" t="n">
+      <c r="H37" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="D38" s="4"/>
-      <c r="E38" s="6" t="n">
+      <c r="D38" s="5"/>
+      <c r="E38" s="7" t="n">
         <v>20000</v>
       </c>
-      <c r="F38" s="4" t="n">
+      <c r="F38" s="5" t="n">
         <v>96332</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G38" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="H38" s="6" t="n">
+      <c r="H38" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="4"/>
-      <c r="E39" s="6" t="n">
+      <c r="D39" s="5"/>
+      <c r="E39" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G39" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="H39" s="6" t="n">
+      <c r="H39" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="42.75" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="6" t="n">
+      <c r="D40" s="5"/>
+      <c r="E40" s="7" t="n">
         <v>17400</v>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="5" t="n">
         <v>84398</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G40" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="H40" s="6" t="n">
+      <c r="H40" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" s="4" t="n">
+      <c r="D41" s="5"/>
+      <c r="E41" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="G41" s="7" t="s">
+      <c r="G41" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="H41" s="6" t="n">
+      <c r="H41" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="D42" s="4"/>
-      <c r="E42" s="6" t="n">
+      <c r="D42" s="5"/>
+      <c r="E42" s="7" t="n">
         <v>20000</v>
       </c>
-      <c r="F42" s="4" t="n">
+      <c r="F42" s="5" t="n">
         <v>96318</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="G42" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="H42" s="6" t="n">
+      <c r="H42" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="4"/>
-      <c r="E43" s="6" t="n">
+      <c r="D43" s="5"/>
+      <c r="E43" s="7" t="n">
         <v>5494</v>
       </c>
-      <c r="F43" s="4" t="n">
+      <c r="F43" s="5" t="n">
         <v>62531</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="H43" s="6" t="n">
+      <c r="H43" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" s="4" t="n">
+      <c r="D44" s="5"/>
+      <c r="E44" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5" t="n">
         <v>34294</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="H44" s="6" t="n">
+      <c r="H44" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C45" s="16" t="s">
+      <c r="C45" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="E45" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G45" s="3" t="s">
+      <c r="E45" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G45" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H45" s="3" t="n">
+      <c r="H45" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C46" s="16" t="s">
+      <c r="C46" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="E46" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" s="3" t="s">
+      <c r="E46" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H46" s="3" t="n">
+      <c r="H46" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C47" s="17" t="s">
+      <c r="C47" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="E47" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G47" s="3" t="s">
+      <c r="E47" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H47" s="3" t="n">
+      <c r="H47" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C48" s="17" t="s">
+      <c r="C48" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="E48" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G48" s="3" t="s">
+      <c r="E48" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H48" s="3" t="n">
+      <c r="H48" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="18" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="17" t="s">
+      <c r="C49" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="D49" s="17"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="17" t="n">
-        <v>1</v>
-      </c>
-      <c r="G49" s="18" t="s">
+      <c r="D49" s="18"/>
+      <c r="E49" s="19"/>
+      <c r="F49" s="18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G49" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="H49" s="3" t="n">
+      <c r="H49" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="E50" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="F50" s="1" t="n">
         <v>7807</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="G50" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="H50" s="3" t="n">
+      <c r="H50" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3" t="n">
+      <c r="G51" s="4"/>
+      <c r="H51" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="6" t="n">
+      <c r="D52" s="5"/>
+      <c r="E52" s="7" t="n">
         <v>5309666</v>
       </c>
-      <c r="F52" s="4" t="n">
+      <c r="F52" s="5" t="n">
         <v>11814</v>
       </c>
-      <c r="G52" s="7" t="s">
+      <c r="G52" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="H52" s="6" t="n">
+      <c r="H52" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="6" t="n">
+      <c r="D53" s="5"/>
+      <c r="E53" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="F53" s="4" t="n">
+      <c r="F53" s="5" t="n">
         <v>715</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G53" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="H53" s="6" t="n">
+      <c r="H53" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C54" s="17" t="s">
         <v>174</v>
       </c>
-      <c r="E54" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="E54" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G54" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H54" s="3" t="n">
+      <c r="H54" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C55" s="16" t="s">
+      <c r="C55" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="E55" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="E55" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G55" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H55" s="3" t="n">
+      <c r="H55" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C56" s="17" t="s">
+      <c r="C56" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="E56" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="F56" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G56" s="3" t="s">
+      <c r="F56" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G56" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H56" s="3" t="n">
+      <c r="H56" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="6" t="n">
+      <c r="D57" s="5"/>
+      <c r="E57" s="7" t="n">
         <v>45</v>
       </c>
-      <c r="F57" s="4" t="n">
+      <c r="F57" s="5" t="n">
         <v>260</v>
       </c>
-      <c r="G57" s="7" t="s">
+      <c r="G57" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="H57" s="6" t="n">
+      <c r="H57" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="6" t="n">
+      <c r="D58" s="5"/>
+      <c r="E58" s="7" t="n">
         <v>3121</v>
       </c>
-      <c r="F58" s="4" t="n">
+      <c r="F58" s="5" t="n">
         <v>50</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="G58" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="H58" s="6" t="n">
+      <c r="H58" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="20" t="n">
+      <c r="D59" s="5"/>
+      <c r="E59" s="21" t="n">
         <v>27030</v>
       </c>
-      <c r="F59" s="4" t="n">
+      <c r="F59" s="5" t="n">
         <v>6967</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="G59" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="H59" s="6" t="n">
+      <c r="H59" s="7" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C60" s="17" t="s">
+      <c r="C60" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="E60" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G60" s="3" t="s">
+      <c r="F60" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G60" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H60" s="3" t="n">
+      <c r="H60" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="6" t="s">
+      <c r="D61" s="5"/>
+      <c r="E61" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="F61" s="4" t="n">
+      <c r="F61" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="G61" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="H61" s="6" t="n">
+      <c r="H61" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C62" s="2" t="s">
+      <c r="C62" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="E62" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="F62" s="0" t="n">
+      <c r="F62" s="1" t="n">
         <v>1052</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="G62" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H62" s="3" t="n">
+      <c r="H62" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F63" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="G63" s="3" t="s">
+      <c r="G63" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H63" s="3" t="n">
+      <c r="H63" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F64" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="G64" s="3" t="s">
+      <c r="G64" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H64" s="3" t="n">
+      <c r="H64" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="F65" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="G65" s="3" t="s">
+      <c r="G65" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H65" s="3" t="n">
+      <c r="H65" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="E66" s="3" t="n">
+      <c r="E66" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F66" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="G66" s="3" t="s">
+      <c r="G66" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="H66" s="3" t="n">
+      <c r="H66" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C67" s="17" t="s">
+      <c r="C67" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="F67" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G67" s="3" t="s">
+      <c r="F67" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H67" s="3" t="n">
+      <c r="H67" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="17" t="s">
+      <c r="C68" s="18" t="s">
         <v>211</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="F68" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G68" s="3" t="s">
+      <c r="F68" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G68" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="H68" s="3" t="n">
+      <c r="H68" s="4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="1" t="n">
         <f aca="false">COUNTA(_xlfn.unique(B80:B180))</f>
         <v>1</v>
       </c>
@@ -2690,7 +2673,7 @@
       <c r="B80" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="C80" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2698,7 +2681,7 @@
       <c r="B81" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="C81" s="1" t="n">
         <f aca="false">C80+1</f>
         <v>2</v>
       </c>
@@ -2707,7 +2690,7 @@
       <c r="B82" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="C82" s="1" t="n">
         <f aca="false">C81+1</f>
         <v>3</v>
       </c>
@@ -2716,7 +2699,7 @@
       <c r="B83" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C83" s="0" t="n">
+      <c r="C83" s="1" t="n">
         <f aca="false">C82+1</f>
         <v>4</v>
       </c>
@@ -2725,7 +2708,7 @@
       <c r="B84" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C84" s="0" t="n">
+      <c r="C84" s="1" t="n">
         <f aca="false">C83+1</f>
         <v>5</v>
       </c>
@@ -2734,7 +2717,7 @@
       <c r="B85" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C85" s="0" t="n">
+      <c r="C85" s="1" t="n">
         <f aca="false">C84+1</f>
         <v>6</v>
       </c>
@@ -2743,7 +2726,7 @@
       <c r="B86" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C86" s="0" t="n">
+      <c r="C86" s="1" t="n">
         <f aca="false">C85+1</f>
         <v>7</v>
       </c>
@@ -2752,7 +2735,7 @@
       <c r="B87" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C87" s="0" t="n">
+      <c r="C87" s="1" t="n">
         <f aca="false">C86+1</f>
         <v>8</v>
       </c>
@@ -2761,7 +2744,7 @@
       <c r="B88" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C88" s="0" t="n">
+      <c r="C88" s="1" t="n">
         <f aca="false">C87+1</f>
         <v>9</v>
       </c>
@@ -2770,7 +2753,7 @@
       <c r="B89" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="C89" s="0" t="n">
+      <c r="C89" s="1" t="n">
         <f aca="false">C88+1</f>
         <v>10</v>
       </c>
@@ -2779,7 +2762,7 @@
       <c r="B90" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C90" s="0" t="n">
+      <c r="C90" s="1" t="n">
         <f aca="false">C89+1</f>
         <v>11</v>
       </c>
@@ -2788,7 +2771,7 @@
       <c r="B91" s="24" t="s">
         <v>56</v>
       </c>
-      <c r="C91" s="0" t="n">
+      <c r="C91" s="1" t="n">
         <f aca="false">C90+1</f>
         <v>12</v>
       </c>
@@ -2797,7 +2780,7 @@
       <c r="B92" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="C92" s="0" t="n">
+      <c r="C92" s="1" t="n">
         <f aca="false">C91+1</f>
         <v>13</v>
       </c>
@@ -2806,7 +2789,7 @@
       <c r="B93" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C93" s="0" t="n">
+      <c r="C93" s="1" t="n">
         <f aca="false">C92+1</f>
         <v>14</v>
       </c>
@@ -2815,7 +2798,7 @@
       <c r="B94" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="C94" s="0" t="n">
+      <c r="C94" s="1" t="n">
         <f aca="false">C93+1</f>
         <v>15</v>
       </c>
@@ -2824,7 +2807,7 @@
       <c r="B95" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C95" s="0" t="n">
+      <c r="C95" s="1" t="n">
         <f aca="false">C94+1</f>
         <v>16</v>
       </c>
@@ -2833,7 +2816,7 @@
       <c r="B96" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="C96" s="0" t="n">
+      <c r="C96" s="1" t="n">
         <f aca="false">C95+1</f>
         <v>17</v>
       </c>
@@ -2842,7 +2825,7 @@
       <c r="B97" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C97" s="0" t="n">
+      <c r="C97" s="1" t="n">
         <f aca="false">C96+1</f>
         <v>18</v>
       </c>
@@ -2851,7 +2834,7 @@
       <c r="B98" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="C98" s="0" t="n">
+      <c r="C98" s="1" t="n">
         <f aca="false">C97+1</f>
         <v>19</v>
       </c>
@@ -2860,7 +2843,7 @@
       <c r="B99" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C99" s="0" t="n">
+      <c r="C99" s="1" t="n">
         <f aca="false">C98+1</f>
         <v>20</v>
       </c>
@@ -2869,7 +2852,7 @@
       <c r="B100" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="C100" s="0" t="n">
+      <c r="C100" s="1" t="n">
         <f aca="false">C99+1</f>
         <v>21</v>
       </c>
@@ -2878,7 +2861,7 @@
       <c r="B101" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C101" s="0" t="n">
+      <c r="C101" s="1" t="n">
         <f aca="false">C100+1</f>
         <v>22</v>
       </c>
@@ -2887,7 +2870,7 @@
       <c r="B102" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="C102" s="0" t="n">
+      <c r="C102" s="1" t="n">
         <f aca="false">C101+1</f>
         <v>23</v>
       </c>
@@ -2896,7 +2879,7 @@
       <c r="B103" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C103" s="0" t="n">
+      <c r="C103" s="1" t="n">
         <f aca="false">C102+1</f>
         <v>24</v>
       </c>
@@ -2905,7 +2888,7 @@
       <c r="B104" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="C104" s="0" t="n">
+      <c r="C104" s="1" t="n">
         <f aca="false">C103+1</f>
         <v>25</v>
       </c>
@@ -2914,7 +2897,7 @@
       <c r="B105" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C105" s="0" t="n">
+      <c r="C105" s="1" t="n">
         <f aca="false">C104+1</f>
         <v>26</v>
       </c>
@@ -2923,7 +2906,7 @@
       <c r="B106" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="C106" s="0" t="n">
+      <c r="C106" s="1" t="n">
         <f aca="false">C105+1</f>
         <v>27</v>
       </c>
@@ -2932,7 +2915,7 @@
       <c r="B107" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="C107" s="0" t="n">
+      <c r="C107" s="1" t="n">
         <f aca="false">C106+1</f>
         <v>28</v>
       </c>
@@ -2941,7 +2924,7 @@
       <c r="B108" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="C108" s="0" t="n">
+      <c r="C108" s="1" t="n">
         <f aca="false">C107+1</f>
         <v>29</v>
       </c>
@@ -2950,7 +2933,7 @@
       <c r="B109" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="C109" s="0" t="n">
+      <c r="C109" s="1" t="n">
         <f aca="false">C108+1</f>
         <v>30</v>
       </c>
@@ -2959,7 +2942,7 @@
       <c r="B110" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="C110" s="0" t="n">
+      <c r="C110" s="1" t="n">
         <f aca="false">C109+1</f>
         <v>31</v>
       </c>
@@ -2968,7 +2951,7 @@
       <c r="B111" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="C111" s="0" t="n">
+      <c r="C111" s="1" t="n">
         <f aca="false">C110+1</f>
         <v>32</v>
       </c>
@@ -2977,7 +2960,7 @@
       <c r="B112" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="C112" s="0" t="n">
+      <c r="C112" s="1" t="n">
         <f aca="false">C111+1</f>
         <v>33</v>
       </c>
@@ -2986,7 +2969,7 @@
       <c r="B113" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="C113" s="0" t="n">
+      <c r="C113" s="1" t="n">
         <f aca="false">C112+1</f>
         <v>34</v>
       </c>
@@ -2995,7 +2978,7 @@
       <c r="B114" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="C114" s="0" t="n">
+      <c r="C114" s="1" t="n">
         <f aca="false">C113+1</f>
         <v>35</v>
       </c>
@@ -3004,7 +2987,7 @@
       <c r="B115" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C115" s="0" t="n">
+      <c r="C115" s="1" t="n">
         <f aca="false">C114+1</f>
         <v>36</v>
       </c>
@@ -3013,7 +2996,7 @@
       <c r="B116" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C116" s="0" t="n">
+      <c r="C116" s="1" t="n">
         <f aca="false">C115+1</f>
         <v>37</v>
       </c>
@@ -3022,7 +3005,7 @@
       <c r="B117" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="C117" s="0" t="n">
+      <c r="C117" s="1" t="n">
         <f aca="false">C116+1</f>
         <v>38</v>
       </c>
@@ -3031,25 +3014,25 @@
       <c r="B118" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="C118" s="0" t="n">
+      <c r="C118" s="1" t="n">
         <f aca="false">C117+1</f>
         <v>39</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="26" t="s">
+      <c r="B119" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="C119" s="0" t="n">
+      <c r="C119" s="1" t="n">
         <f aca="false">C118+1</f>
         <v>40</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="27" t="s">
+      <c r="B120" s="26" t="s">
         <v>171</v>
       </c>
-      <c r="C120" s="0" t="n">
+      <c r="C120" s="1" t="n">
         <f aca="false">C119+1</f>
         <v>41</v>
       </c>
@@ -3058,7 +3041,7 @@
       <c r="B121" s="24" t="s">
         <v>181</v>
       </c>
-      <c r="C121" s="0" t="n">
+      <c r="C121" s="1" t="n">
         <f aca="false">C120+1</f>
         <v>42</v>
       </c>
@@ -3067,7 +3050,7 @@
       <c r="B122" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="C122" s="0" t="n">
+      <c r="C122" s="1" t="n">
         <f aca="false">C121+1</f>
         <v>43</v>
       </c>
@@ -3076,7 +3059,7 @@
       <c r="B123" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="C123" s="0" t="n">
+      <c r="C123" s="1" t="n">
         <f aca="false">C122+1</f>
         <v>44</v>
       </c>

</xml_diff>